<commit_message>
Add formula and test case sample in MasterGalleryKey and MasterGallerySubmission excel sheets
</commit_message>
<xml_diff>
--- a/sample_excel_files/MasterGalleryKey.xlsx
+++ b/sample_excel_files/MasterGalleryKey.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ricardopramanasuranta/Documents/Projects-CMUSV/Fall-2020/18980-GRA/pysheetgrader/sample_excel_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDF895A6-53DC-324E-9775-4755FBE16893}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43F00216-1E6D-364D-B50B-008E53EB6AC7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-20" yWindow="460" windowWidth="28800" windowHeight="17540" activeTab="1" xr2:uid="{6E72627C-1CB6-4848-9B50-C1295434D515}"/>
+    <workbookView xWindow="-20" yWindow="460" windowWidth="28800" windowHeight="17540" activeTab="4" xr2:uid="{6E72627C-1CB6-4848-9B50-C1295434D515}"/>
   </bookViews>
   <sheets>
     <sheet name="SheetGradingOrder" sheetId="1" r:id="rId1"/>
@@ -367,8 +367,238 @@
 </comments>
 </file>
 
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Ricardo Pramana Suranta</author>
+  </authors>
+  <commentList>
+    <comment ref="B3" authorId="0" shapeId="0" xr:uid="{3A92D9DB-F41E-D94C-90F2-6CD76ACF5820}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">rubric:
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> score: 1.5
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> type: formula
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B4" authorId="0" shapeId="0" xr:uid="{DAAD0B80-712C-C441-B2BC-853E4B577A79}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">rubric:
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> score: 1.5
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> type: formula
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B7" authorId="0" shapeId="0" xr:uid="{AAF9CEFF-2DF0-C340-9B67-76233EA5B21B}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">rubric:
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> score: 1
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> type: formula
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B8" authorId="0" shapeId="0" xr:uid="{3CCC1AE5-053B-C649-A73F-F4C7437CBDDA}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">rubric:
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> score: 1.5
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> type: formula
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B9" authorId="0" shapeId="0" xr:uid="{2DD28452-4D0F-454F-B08A-F896EE3CC1D5}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">rubric:
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> score: 1.5
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> type: formula
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">alt_cells:
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> - C10
+</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="28">
   <si>
     <t>Number</t>
   </si>
@@ -446,6 +676,12 @@
   </si>
   <si>
     <t>B9</t>
+  </si>
+  <si>
+    <t>Remember that constant comparison will only compare the formula, not the computed values.</t>
+  </si>
+  <si>
+    <t>&gt; This cell has no rubric, so it won't be processed.</t>
   </si>
 </sst>
 </file>
@@ -855,8 +1091,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A103586-2C0E-0748-80AF-98E299C769E5}">
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="153" zoomScaleNormal="153" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView zoomScale="153" zoomScaleNormal="153" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -964,7 +1200,7 @@
   <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView zoomScale="213" zoomScaleNormal="213" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection sqref="A1:B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1035,37 +1271,181 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EEB70C9E-5A32-AF4F-951C-2DFC686CB197}">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EEB70C9E-5A32-AF4F-951C-2DFC686CB197}">
+  <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView zoomScale="159" zoomScaleNormal="159" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="14.6640625" customWidth="1"/>
+    <col min="2" max="2" width="15.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2">
+        <v>2020</v>
+      </c>
+      <c r="E2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3">
+        <f>B2 / 10</f>
+        <v>202</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4">
+        <f xml:space="preserve">  ROUNDUP(B2 / 100, 0)</f>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7">
+        <f xml:space="preserve"> B6 / 1000</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8">
+        <f>B6 * 3.28084</f>
+        <v>3280.84</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9">
+        <f>B6 * 39.3701</f>
+        <v>39370.1</v>
+      </c>
+      <c r="E9" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C10">
+        <f>B6 * 39.37</f>
+        <v>39370</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9AF83535-20BE-CA43-B82B-2F0E1F118D83}">
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView zoomScale="224" zoomScaleNormal="224" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" zoomScale="224" zoomScaleNormal="224" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add missing changes in MasterGallerKey and MasterGallerySubmission
</commit_message>
<xml_diff>
--- a/sample_excel_files/MasterGalleryKey.xlsx
+++ b/sample_excel_files/MasterGalleryKey.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ricardopramanasuranta/Documents/Projects-CMUSV/Fall-2020/18980-GRA/pysheetgrader/sample_excel_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43F00216-1E6D-364D-B50B-008E53EB6AC7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07F7B98A-9321-8D41-9DDA-986713AB61CE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-20" yWindow="460" windowWidth="28800" windowHeight="17540" activeTab="4" xr2:uid="{6E72627C-1CB6-4848-9B50-C1295434D515}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" activeTab="6" xr2:uid="{6E72627C-1CB6-4848-9B50-C1295434D515}"/>
   </bookViews>
   <sheets>
     <sheet name="SheetGradingOrder" sheetId="1" r:id="rId1"/>
@@ -19,9 +19,9 @@
     <sheet name="Formula Samples" sheetId="3" r:id="rId4"/>
     <sheet name="Formula Samples_CheckOrder" sheetId="6" r:id="rId5"/>
     <sheet name="Test Case Samples" sheetId="4" r:id="rId6"/>
-    <sheet name="Test Cases Samples_CheckOrder" sheetId="7" r:id="rId7"/>
+    <sheet name="Test Case Samples_CheckOrder" sheetId="7" r:id="rId7"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -597,8 +597,360 @@
 </comments>
 </file>
 
+<file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Ricardo Pramana Suranta</author>
+  </authors>
+  <commentList>
+    <comment ref="B5" authorId="0" shapeId="0" xr:uid="{2F37875C-F1FE-DB47-9444-CB9BC8E84C6F}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">rubric:
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> score: 1.5
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> type: test
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">test_cases:
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> default_test:
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">  output: 21
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">  input:
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">   B2: 2020
+   B4: 0
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> custom_rounding_input:
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">   output: 20.2
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">   input:
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">    B2: 2020
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">    B4: 1
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B9" authorId="0" shapeId="0" xr:uid="{D4AA5DAC-07A2-6648-9C78-8C383E30932D}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">rubric:
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> score: 1.5
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> type: test
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">test_cases:
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> default_test:
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">  output: 3280.84
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">  delta: 0.26
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">  input:
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">   B7: 1000
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B10" authorId="0" shapeId="0" xr:uid="{F8B2639D-5638-E240-BF11-8557EDA06127}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">rubric:
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> score: 1.5
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> type: test
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">alt_cells:
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> - C10
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">test_cases:
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> default_test:
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">  output: 39370
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">  input:
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">   B7: 1000</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="35">
   <si>
     <t>Number</t>
   </si>
@@ -633,9 +985,6 @@
     <t>Notes</t>
   </si>
   <si>
-    <t>Remember that constant comparison will only compare the computed value, not the formula.</t>
-  </si>
-  <si>
     <t>Meter</t>
   </si>
   <si>
@@ -678,10 +1027,34 @@
     <t>B9</t>
   </si>
   <si>
-    <t>Remember that constant comparison will only compare the formula, not the computed values.</t>
-  </si>
-  <si>
     <t>&gt; This cell has no rubric, so it won't be processed.</t>
+  </si>
+  <si>
+    <t>Formula comparison will only compare the formula, not the computed values.</t>
+  </si>
+  <si>
+    <t>Constant comparison will only compare the computed value, not the formula.</t>
+  </si>
+  <si>
+    <t>Test case runs are there to handle cases where the formula cannot be simplified, and we want to test different outcomes instead of only the computed value.</t>
+  </si>
+  <si>
+    <t>The test_case rubric will ignore alt_cells.</t>
+  </si>
+  <si>
+    <t>The test case rubric will allow delta on the output.</t>
+  </si>
+  <si>
+    <t>Century Rounder</t>
+  </si>
+  <si>
+    <t>B5</t>
+  </si>
+  <si>
+    <t>All cell references needs to have a value. Multiple test cases are allowed.</t>
+  </si>
+  <si>
+    <t>B10</t>
   </si>
 </sst>
 </file>
@@ -1092,7 +1465,7 @@
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView zoomScale="153" zoomScaleNormal="153" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1120,7 +1493,7 @@
         <v>2020</v>
       </c>
       <c r="E2" t="s">
-        <v>11</v>
+        <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
@@ -1143,7 +1516,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B6">
         <v>1000</v>
@@ -1151,7 +1524,7 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B7">
         <f xml:space="preserve"> B6 / 1000</f>
@@ -1160,26 +1533,26 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B8">
         <f>B6 * 3.28084</f>
         <v>3280.84</v>
       </c>
       <c r="E8" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B9">
         <f>B6 * 39.3701</f>
         <v>39370.1</v>
       </c>
       <c r="E9" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
@@ -1210,7 +1583,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
@@ -1218,7 +1591,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
@@ -1226,7 +1599,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
@@ -1234,7 +1607,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
@@ -1242,7 +1615,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
@@ -1250,7 +1623,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
@@ -1258,7 +1631,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
@@ -1266,7 +1639,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -1280,7 +1653,7 @@
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView zoomScale="159" zoomScaleNormal="159" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1331,7 +1704,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B6">
         <v>1000</v>
@@ -1339,7 +1712,7 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B7">
         <f xml:space="preserve"> B6 / 1000</f>
@@ -1348,7 +1721,7 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B8">
         <f>B6 * 3.28084</f>
@@ -1357,14 +1730,14 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B9">
         <f>B6 * 39.3701</f>
         <v>39370.1</v>
       </c>
       <c r="E9" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
@@ -1375,6 +1748,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
@@ -1383,8 +1757,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9AF83535-20BE-CA43-B82B-2F0E1F118D83}">
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="224" zoomScaleNormal="224" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView zoomScale="224" zoomScaleNormal="224" workbookViewId="0">
+      <selection sqref="A1:B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1394,7 +1768,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
@@ -1402,10 +1776,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
@@ -1413,7 +1787,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
@@ -1421,7 +1795,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
@@ -1429,7 +1803,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
@@ -1437,7 +1811,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
@@ -1445,32 +1819,138 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{064C43C6-5CB5-C440-9F78-B7711421521C}">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{064C43C6-5CB5-C440-9F78-B7711421521C}">
+  <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView zoomScale="187" zoomScaleNormal="187" workbookViewId="0"/>
+    <sheetView zoomScale="187" zoomScaleNormal="187" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="15.1640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2">
+        <v>2020</v>
+      </c>
+      <c r="E2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3">
+        <f>B2 / 10</f>
+        <v>202</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>31</v>
+      </c>
+      <c r="B4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5">
+        <f xml:space="preserve">  ROUNDUP(B2 / 100, B4)</f>
+        <v>21</v>
+      </c>
+      <c r="E5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8">
+        <f xml:space="preserve"> B7 / 1000</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9">
+        <f>B7 * 3.28084</f>
+        <v>3280.84</v>
+      </c>
+      <c r="E9" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10">
+        <f>B7 * 39.3701</f>
+        <v>39370.1</v>
+      </c>
+      <c r="E10" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C11">
+        <f>B7 * 39.37</f>
+        <v>39370</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8290A36-E311-014F-BFC1-47B09A169C19}">
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1480,7 +1960,31 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>18</v>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add Sum comparison to MasterGallery sheets
</commit_message>
<xml_diff>
--- a/sample_excel_files/MasterGalleryKey.xlsx
+++ b/sample_excel_files/MasterGalleryKey.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ricardopramanasuranta/Documents/Projects-CMUSV/Fall-2020/18980-GRA/pysheetgrader/sample_excel_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07F7B98A-9321-8D41-9DDA-986713AB61CE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35A579CC-1644-3341-8A66-847FA97AFE79}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" activeTab="6" xr2:uid="{6E72627C-1CB6-4848-9B50-C1295434D515}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" activeTab="4" xr2:uid="{6E72627C-1CB6-4848-9B50-C1295434D515}"/>
   </bookViews>
   <sheets>
     <sheet name="SheetGradingOrder" sheetId="1" r:id="rId1"/>
@@ -593,6 +593,39 @@
         </r>
       </text>
     </comment>
+    <comment ref="B11" authorId="0" shapeId="0" xr:uid="{B7712E80-D534-ED47-A1EA-2A5A08C12027}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">rubric:
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> score: 2
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> type: formula</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
@@ -950,7 +983,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="37">
   <si>
     <t>Number</t>
   </si>
@@ -1055,6 +1088,12 @@
   </si>
   <si>
     <t>B10</t>
+  </si>
+  <si>
+    <t>Sum</t>
+  </si>
+  <si>
+    <t>B11</t>
   </si>
 </sst>
 </file>
@@ -1650,10 +1689,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EEB70C9E-5A32-AF4F-951C-2DFC686CB197}">
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView zoomScale="159" zoomScaleNormal="159" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1746,6 +1785,15 @@
         <v>39370</v>
       </c>
     </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>35</v>
+      </c>
+      <c r="B11">
+        <f>SUM(B2:B4)</f>
+        <v>2243</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -1755,10 +1803,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9AF83535-20BE-CA43-B82B-2F0E1F118D83}">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView zoomScale="224" zoomScaleNormal="224" workbookViewId="0">
-      <selection sqref="A1:B7"/>
+    <sheetView tabSelected="1" zoomScale="224" zoomScaleNormal="224" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1820,6 +1868,14 @@
       </c>
       <c r="B7" t="s">
         <v>24</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>36</v>
       </c>
     </row>
   </sheetData>
@@ -1949,7 +2005,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8290A36-E311-014F-BFC1-47B09A169C19}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Add further sample for MasterGallery sheets
</commit_message>
<xml_diff>
--- a/sample_excel_files/MasterGalleryKey.xlsx
+++ b/sample_excel_files/MasterGalleryKey.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ricardopramanasuranta/Documents/Projects-CMUSV/Fall-2020/18980-GRA/pysheetgrader/sample_excel_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35A579CC-1644-3341-8A66-847FA97AFE79}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FA53C0D-9C4F-BD42-9D4A-B7CA14F35420}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" activeTab="4" xr2:uid="{6E72627C-1CB6-4848-9B50-C1295434D515}"/>
+    <workbookView xWindow="0" yWindow="480" windowWidth="19200" windowHeight="19440" firstSheet="1" activeTab="3" xr2:uid="{6E72627C-1CB6-4848-9B50-C1295434D515}"/>
   </bookViews>
   <sheets>
     <sheet name="SheetGradingOrder" sheetId="1" r:id="rId1"/>
@@ -626,6 +626,39 @@
         </r>
       </text>
     </comment>
+    <comment ref="B12" authorId="0" shapeId="0" xr:uid="{A60AB632-FF04-DA42-9651-C4D1D0084018}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">rubric:
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> score: 2
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> type: formula</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
@@ -983,7 +1016,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="39">
   <si>
     <t>Number</t>
   </si>
@@ -1094,6 +1127,12 @@
   </si>
   <si>
     <t>B11</t>
+  </si>
+  <si>
+    <t>Sum with extra algebraic calculation</t>
+  </si>
+  <si>
+    <t>B12</t>
   </si>
 </sst>
 </file>
@@ -1689,15 +1728,15 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EEB70C9E-5A32-AF4F-951C-2DFC686CB197}">
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:E12"/>
   <sheetViews>
-    <sheetView zoomScale="159" zoomScaleNormal="159" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView tabSelected="1" zoomScale="159" zoomScaleNormal="159" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="14.6640625" customWidth="1"/>
+    <col min="1" max="1" width="30.5" customWidth="1"/>
     <col min="2" max="2" width="15.6640625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1792,6 +1831,15 @@
       <c r="B11">
         <f>SUM(B2:B4)</f>
         <v>2243</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>37</v>
+      </c>
+      <c r="B12">
+        <f>SUM(B2:B4) + 2</f>
+        <v>2245</v>
       </c>
     </row>
   </sheetData>
@@ -1803,10 +1851,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9AF83535-20BE-CA43-B82B-2F0E1F118D83}">
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="224" zoomScaleNormal="224" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView zoomScale="224" zoomScaleNormal="224" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1876,6 +1924,14 @@
       </c>
       <c r="B8" t="s">
         <v>36</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Implement relative rubric type.
</commit_message>
<xml_diff>
--- a/sample_excel_files/MasterGalleryKey.xlsx
+++ b/sample_excel_files/MasterGalleryKey.xlsx
@@ -1,25 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11213"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ricardopramanasuranta/Documents/Projects-CMUSV/Fall-2020/18980-GRA/pysheetgrader/sample_excel_files/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hanfa/workspace/pysheetgrader/sample_excel_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FA53C0D-9C4F-BD42-9D4A-B7CA14F35420}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF28F187-06C7-6142-8370-B279106ED0B5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="480" windowWidth="19200" windowHeight="19440" firstSheet="1" activeTab="3" xr2:uid="{6E72627C-1CB6-4848-9B50-C1295434D515}"/>
+    <workbookView xWindow="4800" yWindow="520" windowWidth="19200" windowHeight="19440" firstSheet="1" activeTab="2" xr2:uid="{6E72627C-1CB6-4848-9B50-C1295434D515}"/>
   </bookViews>
   <sheets>
     <sheet name="SheetGradingOrder" sheetId="1" r:id="rId1"/>
-    <sheet name="Constant Samples" sheetId="2" r:id="rId2"/>
-    <sheet name="Constant Samples_CheckOrder" sheetId="5" r:id="rId3"/>
-    <sheet name="Formula Samples" sheetId="3" r:id="rId4"/>
-    <sheet name="Formula Samples_CheckOrder" sheetId="6" r:id="rId5"/>
-    <sheet name="Test Case Samples" sheetId="4" r:id="rId6"/>
-    <sheet name="Test Case Samples_CheckOrder" sheetId="7" r:id="rId7"/>
+    <sheet name="Relative Samples_CheckOrder" sheetId="9" r:id="rId2"/>
+    <sheet name="Relative Samples" sheetId="8" r:id="rId3"/>
+    <sheet name="Constant Samples" sheetId="2" r:id="rId4"/>
+    <sheet name="Constant Samples_CheckOrder" sheetId="5" r:id="rId5"/>
+    <sheet name="Formula Samples" sheetId="3" r:id="rId6"/>
+    <sheet name="Formula Samples_CheckOrder" sheetId="6" r:id="rId7"/>
+    <sheet name="Test Case Samples" sheetId="4" r:id="rId8"/>
+    <sheet name="Test Case Samples_CheckOrder" sheetId="7" r:id="rId9"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -42,324 +44,103 @@
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
-    <author>Ricardo Pramana Suranta</author>
+    <author>Microsoft Office User</author>
   </authors>
   <commentList>
-    <comment ref="B2" authorId="0" shapeId="0" xr:uid="{D71AC230-CA0F-6147-8161-BEFBFBB9A788}">
+    <comment ref="A2" authorId="0" shapeId="0" xr:uid="{1383BC69-8C50-784B-BFC3-6F5B3FBA4BD5}">
       <text>
         <r>
           <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">rubric:
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve"> score: 1
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve"> type: constant
-</t>
+            <sz val="18"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>rubric:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="18"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve"> score: 1</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="18"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve"> type: relative</t>
         </r>
       </text>
     </comment>
-    <comment ref="B3" authorId="0" shapeId="0" xr:uid="{BADCDE6D-B1E6-6247-B944-057D3FE92399}">
+    <comment ref="A3" authorId="0" shapeId="0" xr:uid="{1453B0C4-5752-114C-87AA-DA9334CCCE20}">
       <text>
         <r>
           <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">rubric:
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve"> score: 1.5
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve"> type: constant
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
+            <sz val="18"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t>rubric:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
           </rPr>
           <t xml:space="preserve">
 </t>
         </r>
-      </text>
-    </comment>
-    <comment ref="B4" authorId="0" shapeId="0" xr:uid="{257D5320-BF9E-C746-BB6A-24028FC20CDF}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">rubric:
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve"> score: 1.5
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve"> type: constant
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
+        <r>
+          <rPr>
+            <sz val="18"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t xml:space="preserve"> score: 1</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
           </rPr>
           <t xml:space="preserve">
 </t>
         </r>
-      </text>
-    </comment>
-    <comment ref="B6" authorId="0" shapeId="0" xr:uid="{382D2601-E60D-AF41-9112-5E34159E9F09}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">rubric:
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve"> score: 1
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve"> type: constant
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B7" authorId="0" shapeId="0" xr:uid="{7B36EB09-5FE5-7F4C-90C3-F4B2560DAA48}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">rubric:
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve"> score: 1
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve"> type: constant
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B8" authorId="0" shapeId="0" xr:uid="{D0CAA4B1-7F8C-8545-8917-42FD070A0506}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">rubric:
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve"> score: 1.5
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve"> type: constant
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve"> delta: 0.26
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B9" authorId="0" shapeId="0" xr:uid="{D0987F27-B842-E648-8826-7FE8512871FF}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">rubric:
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve"> score: 1.5
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve"> type: constant
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">alt_cells:
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve"> - C10
-</t>
+        <r>
+          <rPr>
+            <sz val="18"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t xml:space="preserve"> type: relative</t>
         </r>
       </text>
     </comment>
@@ -373,7 +154,7 @@
     <author>Ricardo Pramana Suranta</author>
   </authors>
   <commentList>
-    <comment ref="B3" authorId="0" shapeId="0" xr:uid="{3A92D9DB-F41E-D94C-90F2-6CD76ACF5820}">
+    <comment ref="B2" authorId="0" shapeId="0" xr:uid="{D71AC230-CA0F-6147-8161-BEFBFBB9A788}">
       <text>
         <r>
           <rPr>
@@ -392,32 +173,22 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t xml:space="preserve"> score: 1.5
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve"> type: formula
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
+          <t xml:space="preserve"> score: 1
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> type: constant
 </t>
         </r>
       </text>
     </comment>
-    <comment ref="B4" authorId="0" shapeId="0" xr:uid="{DAAD0B80-712C-C441-B2BC-853E4B577A79}">
+    <comment ref="B3" authorId="0" shapeId="0" xr:uid="{BADCDE6D-B1E6-6247-B944-057D3FE92399}">
       <text>
         <r>
           <rPr>
@@ -446,7 +217,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t xml:space="preserve"> type: formula
+          <t xml:space="preserve"> type: constant
 </t>
         </r>
         <r>
@@ -461,7 +232,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B7" authorId="0" shapeId="0" xr:uid="{AAF9CEFF-2DF0-C340-9B67-76233EA5B21B}">
+    <comment ref="B4" authorId="0" shapeId="0" xr:uid="{257D5320-BF9E-C746-BB6A-24028FC20CDF}">
       <text>
         <r>
           <rPr>
@@ -480,17 +251,17 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t xml:space="preserve"> score: 1
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve"> type: formula
+          <t xml:space="preserve"> score: 1.5
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> type: constant
 </t>
         </r>
         <r>
@@ -505,7 +276,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B8" authorId="0" shapeId="0" xr:uid="{3CCC1AE5-053B-C649-A73F-F4C7437CBDDA}">
+    <comment ref="B6" authorId="0" shapeId="0" xr:uid="{382D2601-E60D-AF41-9112-5E34159E9F09}">
       <text>
         <r>
           <rPr>
@@ -524,22 +295,32 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t xml:space="preserve"> score: 1.5
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve"> type: formula
+          <t xml:space="preserve"> score: 1
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> type: constant
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
 </t>
         </r>
       </text>
     </comment>
-    <comment ref="B9" authorId="0" shapeId="0" xr:uid="{2DD28452-4D0F-454F-B08A-F896EE3CC1D5}">
+    <comment ref="B7" authorId="0" shapeId="0" xr:uid="{7B36EB09-5FE5-7F4C-90C3-F4B2560DAA48}">
       <text>
         <r>
           <rPr>
@@ -558,42 +339,32 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t xml:space="preserve"> score: 1.5
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve"> type: formula
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">alt_cells:
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve"> - C10
+          <t xml:space="preserve"> score: 1
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> type: constant
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
 </t>
         </r>
       </text>
     </comment>
-    <comment ref="B11" authorId="0" shapeId="0" xr:uid="{B7712E80-D534-ED47-A1EA-2A5A08C12027}">
+    <comment ref="B8" authorId="0" shapeId="0" xr:uid="{D0CAA4B1-7F8C-8545-8917-42FD070A0506}">
       <text>
         <r>
           <rPr>
@@ -612,21 +383,42 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t xml:space="preserve"> score: 2
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve"> type: formula</t>
+          <t xml:space="preserve"> score: 1.5
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> type: constant
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> delta: 0.26
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
         </r>
       </text>
     </comment>
-    <comment ref="B12" authorId="0" shapeId="0" xr:uid="{A60AB632-FF04-DA42-9651-C4D1D0084018}">
+    <comment ref="B9" authorId="0" shapeId="0" xr:uid="{D0987F27-B842-E648-8826-7FE8512871FF}">
       <text>
         <r>
           <rPr>
@@ -645,17 +437,38 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t xml:space="preserve"> score: 2
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve"> type: formula</t>
+          <t xml:space="preserve"> score: 1.5
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> type: constant
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">alt_cells:
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> - C10
+</t>
         </r>
       </text>
     </comment>
@@ -669,6 +482,302 @@
     <author>Ricardo Pramana Suranta</author>
   </authors>
   <commentList>
+    <comment ref="B3" authorId="0" shapeId="0" xr:uid="{3A92D9DB-F41E-D94C-90F2-6CD76ACF5820}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">rubric:
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> score: 1.5
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> type: formula
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B4" authorId="0" shapeId="0" xr:uid="{DAAD0B80-712C-C441-B2BC-853E4B577A79}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">rubric:
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> score: 1.5
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> type: formula
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B7" authorId="0" shapeId="0" xr:uid="{AAF9CEFF-2DF0-C340-9B67-76233EA5B21B}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">rubric:
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> score: 1
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> type: formula
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B8" authorId="0" shapeId="0" xr:uid="{3CCC1AE5-053B-C649-A73F-F4C7437CBDDA}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">rubric:
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> score: 1.5
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> type: formula
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B9" authorId="0" shapeId="0" xr:uid="{2DD28452-4D0F-454F-B08A-F896EE3CC1D5}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">rubric:
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> score: 1.5
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> type: formula
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">alt_cells:
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> - C10
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B11" authorId="0" shapeId="0" xr:uid="{B7712E80-D534-ED47-A1EA-2A5A08C12027}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">rubric:
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> score: 2
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> type: formula</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B12" authorId="0" shapeId="0" xr:uid="{A60AB632-FF04-DA42-9651-C4D1D0084018}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">rubric:
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> score: 2
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> type: formula</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments4.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Ricardo Pramana Suranta</author>
+  </authors>
+  <commentList>
     <comment ref="B5" authorId="0" shapeId="0" xr:uid="{2F37875C-F1FE-DB47-9444-CB9BC8E84C6F}">
       <text>
         <r>
@@ -1016,7 +1125,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="45">
   <si>
     <t>Number</t>
   </si>
@@ -1133,13 +1242,31 @@
   </si>
   <si>
     <t>B12</t>
+  </si>
+  <si>
+    <t>Relative Samples</t>
+  </si>
+  <si>
+    <t>Formulas</t>
+  </si>
+  <si>
+    <t>A2</t>
+  </si>
+  <si>
+    <t>// student is correct 3003 = 1001 + 2002</t>
+  </si>
+  <si>
+    <t>// student is incorrect 4005 != 2002 + 2002</t>
+  </si>
+  <si>
+    <t>A3</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1152,6 +1279,28 @@
       <color rgb="FF000000"/>
       <name val="Tahoma"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="2">
@@ -1490,10 +1639,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{713B2A36-CAF8-2349-917C-6D8074132DA3}">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1533,17 +1682,119 @@
         <v>4</v>
       </c>
     </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>39</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05739818-17B0-D842-BB6C-69A1E595FDFD}">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B5E91EC-3DFF-1543-8E9D-3526C440EDB3}">
+  <dimension ref="A1:D3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="13.1640625" customWidth="1"/>
+    <col min="4" max="4" width="39.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <f>B2+C2</f>
+        <v>300</v>
+      </c>
+      <c r="B2">
+        <v>100</v>
+      </c>
+      <c r="C2">
+        <v>200</v>
+      </c>
+      <c r="D2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <f>B3+C3</f>
+        <v>300</v>
+      </c>
+      <c r="B3">
+        <v>100</v>
+      </c>
+      <c r="C3">
+        <v>200</v>
+      </c>
+      <c r="D3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A103586-2C0E-0748-80AF-98E299C769E5}">
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView zoomScale="153" zoomScaleNormal="153" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1646,7 +1897,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71EABA77-C8A8-0247-A6AC-2452B8B329D1}">
   <dimension ref="A1:B8"/>
   <sheetViews>
@@ -1726,12 +1977,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EEB70C9E-5A32-AF4F-951C-2DFC686CB197}">
   <dimension ref="A1:E12"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="159" zoomScaleNormal="159" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView zoomScale="108" zoomScaleNormal="108" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1849,7 +2100,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9AF83535-20BE-CA43-B82B-2F0E1F118D83}">
   <dimension ref="A1:C9"/>
   <sheetViews>
@@ -1940,7 +2191,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{064C43C6-5CB5-C440-9F78-B7711421521C}">
   <dimension ref="A1:E11"/>
   <sheetViews>
@@ -2057,7 +2308,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8290A36-E311-014F-BFC1-47B09A169C19}">
   <dimension ref="A1:B4"/>
   <sheetViews>

</xml_diff>

<commit_message>
Refactor formula transform logic into transform_excel_formula_to_sympy.
</commit_message>
<xml_diff>
--- a/sample_excel_files/MasterGalleryKey.xlsx
+++ b/sample_excel_files/MasterGalleryKey.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hanfa/workspace/pysheetgrader/sample_excel_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF28F187-06C7-6142-8370-B279106ED0B5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD130529-88FF-6C49-8DC1-559FCF4B44D6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4800" yWindow="520" windowWidth="19200" windowHeight="19440" firstSheet="1" activeTab="2" xr2:uid="{6E72627C-1CB6-4848-9B50-C1295434D515}"/>
+    <workbookView xWindow="-26140" yWindow="800" windowWidth="19200" windowHeight="19440" activeTab="2" xr2:uid="{6E72627C-1CB6-4848-9B50-C1295434D515}"/>
   </bookViews>
   <sheets>
     <sheet name="SheetGradingOrder" sheetId="1" r:id="rId1"/>
@@ -144,6 +144,52 @@
         </r>
       </text>
     </comment>
+    <comment ref="A6" authorId="0" shapeId="0" xr:uid="{7B5C625D-8CE9-4640-8FCC-8F3C47D8E7DB}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="18"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t>rubric:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="18"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t xml:space="preserve"> score: 1</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="18"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t xml:space="preserve"> type: relative</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
@@ -1125,7 +1171,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="48">
   <si>
     <t>Number</t>
   </si>
@@ -1260,6 +1306,15 @@
   </si>
   <si>
     <t>A3</t>
+  </si>
+  <si>
+    <t>Complex formula</t>
+  </si>
+  <si>
+    <t>ok</t>
+  </si>
+  <si>
+    <t>A6</t>
   </si>
 </sst>
 </file>
@@ -1340,6 +1395,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1642,7 +1701,7 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="A5" sqref="A5:B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1697,10 +1756,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05739818-17B0-D842-BB6C-69A1E595FDFD}">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1729,6 +1788,14 @@
         <v>44</v>
       </c>
     </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>47</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1736,15 +1803,15 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B5E91EC-3DFF-1543-8E9D-3526C440EDB3}">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="13.1640625" customWidth="1"/>
+    <col min="1" max="1" width="17" customWidth="1"/>
     <col min="4" max="4" width="39.5" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1781,6 +1848,26 @@
       </c>
       <c r="D3" t="s">
         <v>43</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <f xml:space="preserve"> IF(B6="ok",C6,D6)</f>
+        <v>100</v>
+      </c>
+      <c r="B6" t="s">
+        <v>46</v>
+      </c>
+      <c r="C6">
+        <v>100</v>
+      </c>
+      <c r="D6">
+        <v>200</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Allow alt_cells for the relative formula type.
</commit_message>
<xml_diff>
--- a/sample_excel_files/MasterGalleryKey.xlsx
+++ b/sample_excel_files/MasterGalleryKey.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hanfa/workspace/pysheetgrader/sample_excel_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD130529-88FF-6C49-8DC1-559FCF4B44D6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82623DD3-7229-7242-894A-1BC876834912}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-26140" yWindow="800" windowWidth="19200" windowHeight="19440" activeTab="2" xr2:uid="{6E72627C-1CB6-4848-9B50-C1295434D515}"/>
+    <workbookView xWindow="-37320" yWindow="1320" windowWidth="19200" windowHeight="19440" firstSheet="1" activeTab="2" xr2:uid="{6E72627C-1CB6-4848-9B50-C1295434D515}"/>
   </bookViews>
   <sheets>
     <sheet name="SheetGradingOrder" sheetId="1" r:id="rId1"/>
@@ -144,6 +144,147 @@
         </r>
       </text>
     </comment>
+    <comment ref="A4" authorId="0" shapeId="0" xr:uid="{22A2E076-4C02-4B49-A522-36472950712A}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="18"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>rubric:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="18"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve"> score: 1</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="18"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve"> type: relative
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="18"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve"> delta: 5</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A5" authorId="0" shapeId="0" xr:uid="{92A0F7C2-1E9D-8145-B4B7-0026CEA5BAE1}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="18"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>rubric:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="18"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve"> score: 1</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="18"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve"> type: relative</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="18"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">alt_cells:
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="18"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve"> - F10</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="A6" authorId="0" shapeId="0" xr:uid="{7B5C625D-8CE9-4640-8FCC-8F3C47D8E7DB}">
       <text>
         <r>
@@ -1171,7 +1312,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="51">
   <si>
     <t>Number</t>
   </si>
@@ -1308,13 +1449,22 @@
     <t>A3</t>
   </si>
   <si>
-    <t>Complex formula</t>
-  </si>
-  <si>
     <t>ok</t>
   </si>
   <si>
     <t>A6</t>
+  </si>
+  <si>
+    <t>A4</t>
+  </si>
+  <si>
+    <t>A5</t>
+  </si>
+  <si>
+    <t>// alt cells for being more tolerant</t>
+  </si>
+  <si>
+    <t>// delta for being more tolerant</t>
   </si>
 </sst>
 </file>
@@ -1756,10 +1906,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05739818-17B0-D842-BB6C-69A1E595FDFD}">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1796,6 +1946,22 @@
         <v>47</v>
       </c>
     </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>46</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1803,10 +1969,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B5E91EC-3DFF-1543-8E9D-3526C440EDB3}">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1815,12 +1981,12 @@
     <col min="4" max="4" width="39.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2">
         <f>B2+C2</f>
         <v>300</v>
@@ -1835,7 +2001,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3">
         <f>B3+C3</f>
         <v>300</v>
@@ -1850,24 +2016,54 @@
         <v>43</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <f>B4+C4</f>
+        <v>300</v>
+      </c>
+      <c r="B4">
+        <v>100</v>
+      </c>
+      <c r="C4">
+        <v>200</v>
+      </c>
+      <c r="D4" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <f>B5+C5</f>
+        <v>300</v>
+      </c>
+      <c r="B5">
+        <v>100</v>
+      </c>
+      <c r="C5">
+        <v>200</v>
+      </c>
+      <c r="D5" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6">
         <f xml:space="preserve"> IF(B6="ok",C6,D6)</f>
         <v>100</v>
       </c>
       <c r="B6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C6">
         <v>100</v>
       </c>
       <c r="D6">
         <v>200</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F10">
+        <v>8888</v>
       </c>
     </row>
   </sheetData>
@@ -1881,7 +2077,7 @@
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView zoomScale="153" zoomScaleNormal="153" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Implement a new variant of relative formula type that only accept formula cell (i.e. not hardcoded constant)
</commit_message>
<xml_diff>
--- a/sample_excel_files/MasterGalleryKey.xlsx
+++ b/sample_excel_files/MasterGalleryKey.xlsx
@@ -8,20 +8,22 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hanfa/workspace/pysheetgrader/sample_excel_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82623DD3-7229-7242-894A-1BC876834912}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD3DCD68-785F-6145-9329-0476F14CBB7A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-37320" yWindow="1320" windowWidth="19200" windowHeight="19440" firstSheet="1" activeTab="2" xr2:uid="{6E72627C-1CB6-4848-9B50-C1295434D515}"/>
+    <workbookView xWindow="-37320" yWindow="1320" windowWidth="19200" windowHeight="19440" firstSheet="1" activeTab="3" xr2:uid="{6E72627C-1CB6-4848-9B50-C1295434D515}"/>
   </bookViews>
   <sheets>
     <sheet name="SheetGradingOrder" sheetId="1" r:id="rId1"/>
     <sheet name="Relative Samples_CheckOrder" sheetId="9" r:id="rId2"/>
-    <sheet name="Relative Samples" sheetId="8" r:id="rId3"/>
-    <sheet name="Constant Samples" sheetId="2" r:id="rId4"/>
-    <sheet name="Constant Samples_CheckOrder" sheetId="5" r:id="rId5"/>
-    <sheet name="Formula Samples" sheetId="3" r:id="rId6"/>
-    <sheet name="Formula Samples_CheckOrder" sheetId="6" r:id="rId7"/>
-    <sheet name="Test Case Samples" sheetId="4" r:id="rId8"/>
-    <sheet name="Test Case Samples_CheckOrder" sheetId="7" r:id="rId9"/>
+    <sheet name="RelativeF Samples_CheckOrder" sheetId="10" r:id="rId3"/>
+    <sheet name="RelativeF Samples" sheetId="11" r:id="rId4"/>
+    <sheet name="Relative Samples" sheetId="8" r:id="rId5"/>
+    <sheet name="Constant Samples" sheetId="2" r:id="rId6"/>
+    <sheet name="Constant Samples_CheckOrder" sheetId="5" r:id="rId7"/>
+    <sheet name="Formula Samples" sheetId="3" r:id="rId8"/>
+    <sheet name="Formula Samples_CheckOrder" sheetId="6" r:id="rId9"/>
+    <sheet name="Test Case Samples" sheetId="4" r:id="rId10"/>
+    <sheet name="Test Case Samples_CheckOrder" sheetId="7" r:id="rId11"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -47,14 +49,13 @@
     <author>Microsoft Office User</author>
   </authors>
   <commentList>
-    <comment ref="A2" authorId="0" shapeId="0" xr:uid="{1383BC69-8C50-784B-BFC3-6F5B3FBA4BD5}">
+    <comment ref="A2" authorId="0" shapeId="0" xr:uid="{4D1CCE99-8A95-4442-85F1-754578DBE703}">
       <text>
         <r>
           <rPr>
             <sz val="18"/>
             <color rgb="FF000000"/>
             <rFont val="Calibri"/>
-            <scheme val="minor"/>
           </rPr>
           <t>rubric:</t>
         </r>
@@ -63,7 +64,6 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Calibri"/>
-            <scheme val="minor"/>
           </rPr>
           <t xml:space="preserve">
 </t>
@@ -73,7 +73,6 @@
             <sz val="18"/>
             <color rgb="FF000000"/>
             <rFont val="Calibri"/>
-            <scheme val="minor"/>
           </rPr>
           <t xml:space="preserve"> score: 1</t>
         </r>
@@ -82,7 +81,6 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Calibri"/>
-            <scheme val="minor"/>
           </rPr>
           <t xml:space="preserve">
 </t>
@@ -92,13 +90,12 @@
             <sz val="18"/>
             <color rgb="FF000000"/>
             <rFont val="Calibri"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t xml:space="preserve"> type: relative</t>
+          </rPr>
+          <t xml:space="preserve"> type: relative_f</t>
         </r>
       </text>
     </comment>
-    <comment ref="A3" authorId="0" shapeId="0" xr:uid="{1453B0C4-5752-114C-87AA-DA9334CCCE20}">
+    <comment ref="A3" authorId="0" shapeId="0" xr:uid="{DFB19857-F8D2-0549-8FAD-3F09B05D6F7F}">
       <text>
         <r>
           <rPr>
@@ -140,18 +137,17 @@
             <color rgb="FF000000"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t xml:space="preserve"> type: relative</t>
+          <t xml:space="preserve"> type: relative_f</t>
         </r>
       </text>
     </comment>
-    <comment ref="A4" authorId="0" shapeId="0" xr:uid="{22A2E076-4C02-4B49-A522-36472950712A}">
+    <comment ref="A4" authorId="0" shapeId="0" xr:uid="{6625B3A2-7060-E14A-8CAD-A710F9425989}">
       <text>
         <r>
           <rPr>
             <sz val="18"/>
             <color rgb="FF000000"/>
             <rFont val="Calibri"/>
-            <scheme val="minor"/>
           </rPr>
           <t>rubric:</t>
         </r>
@@ -160,7 +156,6 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Calibri"/>
-            <scheme val="minor"/>
           </rPr>
           <t xml:space="preserve">
 </t>
@@ -170,7 +165,6 @@
             <sz val="18"/>
             <color rgb="FF000000"/>
             <rFont val="Calibri"/>
-            <scheme val="minor"/>
           </rPr>
           <t xml:space="preserve"> score: 1</t>
         </r>
@@ -179,7 +173,6 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Calibri"/>
-            <scheme val="minor"/>
           </rPr>
           <t xml:space="preserve">
 </t>
@@ -189,30 +182,27 @@
             <sz val="18"/>
             <color rgb="FF000000"/>
             <rFont val="Calibri"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t xml:space="preserve"> type: relative
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="18"/>
-            <color rgb="FF000000"/>
-            <rFont val="Calibri"/>
-            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve"> type: relative_f
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="18"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
           </rPr>
           <t xml:space="preserve"> delta: 5</t>
         </r>
       </text>
     </comment>
-    <comment ref="A5" authorId="0" shapeId="0" xr:uid="{92A0F7C2-1E9D-8145-B4B7-0026CEA5BAE1}">
+    <comment ref="A5" authorId="0" shapeId="0" xr:uid="{03774356-5573-6340-98D9-BF6F67EE5C0B}">
       <text>
         <r>
           <rPr>
             <sz val="18"/>
             <color rgb="FF000000"/>
             <rFont val="Calibri"/>
-            <scheme val="minor"/>
           </rPr>
           <t>rubric:</t>
         </r>
@@ -221,7 +211,6 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Calibri"/>
-            <scheme val="minor"/>
           </rPr>
           <t xml:space="preserve">
 </t>
@@ -231,7 +220,6 @@
             <sz val="18"/>
             <color rgb="FF000000"/>
             <rFont val="Calibri"/>
-            <scheme val="minor"/>
           </rPr>
           <t xml:space="preserve"> score: 1</t>
         </r>
@@ -240,7 +228,6 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Calibri"/>
-            <scheme val="minor"/>
           </rPr>
           <t xml:space="preserve">
 </t>
@@ -250,16 +237,14 @@
             <sz val="18"/>
             <color rgb="FF000000"/>
             <rFont val="Calibri"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t xml:space="preserve"> type: relative</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Calibri"/>
-            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve"> type: relative_f</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
           </rPr>
           <t xml:space="preserve">
 </t>
@@ -269,7 +254,6 @@
             <sz val="18"/>
             <color rgb="FF000000"/>
             <rFont val="Calibri"/>
-            <scheme val="minor"/>
           </rPr>
           <t xml:space="preserve">alt_cells:
 </t>
@@ -279,55 +263,8 @@
             <sz val="18"/>
             <color rgb="FF000000"/>
             <rFont val="Calibri"/>
-            <scheme val="minor"/>
           </rPr>
           <t xml:space="preserve"> - F10</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="A6" authorId="0" shapeId="0" xr:uid="{7B5C625D-8CE9-4640-8FCC-8F3C47D8E7DB}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="18"/>
-            <color rgb="FF000000"/>
-            <rFont val="Calibri"/>
-          </rPr>
-          <t>rubric:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Calibri"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="18"/>
-            <color rgb="FF000000"/>
-            <rFont val="Calibri"/>
-          </rPr>
-          <t xml:space="preserve"> score: 1</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Calibri"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="18"/>
-            <color rgb="FF000000"/>
-            <rFont val="Calibri"/>
-          </rPr>
-          <t xml:space="preserve"> type: relative</t>
         </r>
       </text>
     </comment>
@@ -338,324 +275,271 @@
 <file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
-    <author>Ricardo Pramana Suranta</author>
+    <author>Microsoft Office User</author>
   </authors>
   <commentList>
-    <comment ref="B2" authorId="0" shapeId="0" xr:uid="{D71AC230-CA0F-6147-8161-BEFBFBB9A788}">
+    <comment ref="A2" authorId="0" shapeId="0" xr:uid="{1383BC69-8C50-784B-BFC3-6F5B3FBA4BD5}">
       <text>
         <r>
           <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">rubric:
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve"> score: 1
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve"> type: constant
-</t>
+            <sz val="18"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t>rubric:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="18"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t xml:space="preserve"> score: 1</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="18"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t xml:space="preserve"> type: relative</t>
         </r>
       </text>
     </comment>
-    <comment ref="B3" authorId="0" shapeId="0" xr:uid="{BADCDE6D-B1E6-6247-B944-057D3FE92399}">
+    <comment ref="A3" authorId="0" shapeId="0" xr:uid="{1453B0C4-5752-114C-87AA-DA9334CCCE20}">
       <text>
         <r>
           <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">rubric:
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve"> score: 1.5
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve"> type: constant
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
+            <sz val="18"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t>rubric:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
           </rPr>
           <t xml:space="preserve">
 </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="18"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t xml:space="preserve"> score: 1</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="18"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t xml:space="preserve"> type: relative</t>
         </r>
       </text>
     </comment>
-    <comment ref="B4" authorId="0" shapeId="0" xr:uid="{257D5320-BF9E-C746-BB6A-24028FC20CDF}">
+    <comment ref="A4" authorId="0" shapeId="0" xr:uid="{22A2E076-4C02-4B49-A522-36472950712A}">
       <text>
         <r>
           <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">rubric:
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve"> score: 1.5
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve"> type: constant
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
+            <sz val="18"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t>rubric:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
           </rPr>
           <t xml:space="preserve">
 </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="18"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t xml:space="preserve"> score: 1</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="18"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t xml:space="preserve"> type: relative
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="18"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t xml:space="preserve"> delta: 5</t>
         </r>
       </text>
     </comment>
-    <comment ref="B6" authorId="0" shapeId="0" xr:uid="{382D2601-E60D-AF41-9112-5E34159E9F09}">
+    <comment ref="A5" authorId="0" shapeId="0" xr:uid="{92A0F7C2-1E9D-8145-B4B7-0026CEA5BAE1}">
       <text>
         <r>
           <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">rubric:
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve"> score: 1
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve"> type: constant
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
+            <sz val="18"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t>rubric:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
           </rPr>
           <t xml:space="preserve">
 </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="18"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t xml:space="preserve"> score: 1</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="18"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t xml:space="preserve"> type: relative</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="18"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t xml:space="preserve">alt_cells:
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="18"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t xml:space="preserve"> - F10</t>
         </r>
       </text>
     </comment>
-    <comment ref="B7" authorId="0" shapeId="0" xr:uid="{7B36EB09-5FE5-7F4C-90C3-F4B2560DAA48}">
+    <comment ref="A6" authorId="0" shapeId="0" xr:uid="{7B5C625D-8CE9-4640-8FCC-8F3C47D8E7DB}">
       <text>
         <r>
           <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">rubric:
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve"> score: 1
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve"> type: constant
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
+            <sz val="18"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t>rubric:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
           </rPr>
           <t xml:space="preserve">
 </t>
         </r>
-      </text>
-    </comment>
-    <comment ref="B8" authorId="0" shapeId="0" xr:uid="{D0CAA4B1-7F8C-8545-8917-42FD070A0506}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">rubric:
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve"> score: 1.5
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve"> type: constant
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve"> delta: 0.26
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
+        <r>
+          <rPr>
+            <sz val="18"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t xml:space="preserve"> score: 1</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
           </rPr>
           <t xml:space="preserve">
 </t>
         </r>
-      </text>
-    </comment>
-    <comment ref="B9" authorId="0" shapeId="0" xr:uid="{D0987F27-B842-E648-8826-7FE8512871FF}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">rubric:
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve"> score: 1.5
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve"> type: constant
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">alt_cells:
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve"> - C10
-</t>
+        <r>
+          <rPr>
+            <sz val="18"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t xml:space="preserve"> type: relative</t>
         </r>
       </text>
     </comment>
@@ -669,7 +553,7 @@
     <author>Ricardo Pramana Suranta</author>
   </authors>
   <commentList>
-    <comment ref="B3" authorId="0" shapeId="0" xr:uid="{3A92D9DB-F41E-D94C-90F2-6CD76ACF5820}">
+    <comment ref="B2" authorId="0" shapeId="0" xr:uid="{D71AC230-CA0F-6147-8161-BEFBFBB9A788}">
       <text>
         <r>
           <rPr>
@@ -688,32 +572,22 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t xml:space="preserve"> score: 1.5
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve"> type: formula
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
+          <t xml:space="preserve"> score: 1
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> type: constant
 </t>
         </r>
       </text>
     </comment>
-    <comment ref="B4" authorId="0" shapeId="0" xr:uid="{DAAD0B80-712C-C441-B2BC-853E4B577A79}">
+    <comment ref="B3" authorId="0" shapeId="0" xr:uid="{BADCDE6D-B1E6-6247-B944-057D3FE92399}">
       <text>
         <r>
           <rPr>
@@ -742,7 +616,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t xml:space="preserve"> type: formula
+          <t xml:space="preserve"> type: constant
 </t>
         </r>
         <r>
@@ -757,7 +631,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B7" authorId="0" shapeId="0" xr:uid="{AAF9CEFF-2DF0-C340-9B67-76233EA5B21B}">
+    <comment ref="B4" authorId="0" shapeId="0" xr:uid="{257D5320-BF9E-C746-BB6A-24028FC20CDF}">
       <text>
         <r>
           <rPr>
@@ -776,17 +650,17 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t xml:space="preserve"> score: 1
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve"> type: formula
+          <t xml:space="preserve"> score: 1.5
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> type: constant
 </t>
         </r>
         <r>
@@ -801,7 +675,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B8" authorId="0" shapeId="0" xr:uid="{3CCC1AE5-053B-C649-A73F-F4C7437CBDDA}">
+    <comment ref="B6" authorId="0" shapeId="0" xr:uid="{382D2601-E60D-AF41-9112-5E34159E9F09}">
       <text>
         <r>
           <rPr>
@@ -820,22 +694,32 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t xml:space="preserve"> score: 1.5
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve"> type: formula
+          <t xml:space="preserve"> score: 1
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> type: constant
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
 </t>
         </r>
       </text>
     </comment>
-    <comment ref="B9" authorId="0" shapeId="0" xr:uid="{2DD28452-4D0F-454F-B08A-F896EE3CC1D5}">
+    <comment ref="B7" authorId="0" shapeId="0" xr:uid="{7B36EB09-5FE5-7F4C-90C3-F4B2560DAA48}">
       <text>
         <r>
           <rPr>
@@ -854,42 +738,32 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t xml:space="preserve"> score: 1.5
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve"> type: formula
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">alt_cells:
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve"> - C10
+          <t xml:space="preserve"> score: 1
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> type: constant
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
 </t>
         </r>
       </text>
     </comment>
-    <comment ref="B11" authorId="0" shapeId="0" xr:uid="{B7712E80-D534-ED47-A1EA-2A5A08C12027}">
+    <comment ref="B8" authorId="0" shapeId="0" xr:uid="{D0CAA4B1-7F8C-8545-8917-42FD070A0506}">
       <text>
         <r>
           <rPr>
@@ -908,21 +782,42 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t xml:space="preserve"> score: 2
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve"> type: formula</t>
+          <t xml:space="preserve"> score: 1.5
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> type: constant
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> delta: 0.26
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
         </r>
       </text>
     </comment>
-    <comment ref="B12" authorId="0" shapeId="0" xr:uid="{A60AB632-FF04-DA42-9651-C4D1D0084018}">
+    <comment ref="B9" authorId="0" shapeId="0" xr:uid="{D0987F27-B842-E648-8826-7FE8512871FF}">
       <text>
         <r>
           <rPr>
@@ -941,17 +836,38 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t xml:space="preserve"> score: 2
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve"> type: formula</t>
+          <t xml:space="preserve"> score: 1.5
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> type: constant
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">alt_cells:
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> - C10
+</t>
         </r>
       </text>
     </comment>
@@ -965,6 +881,302 @@
     <author>Ricardo Pramana Suranta</author>
   </authors>
   <commentList>
+    <comment ref="B3" authorId="0" shapeId="0" xr:uid="{3A92D9DB-F41E-D94C-90F2-6CD76ACF5820}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">rubric:
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> score: 1.5
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> type: formula
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B4" authorId="0" shapeId="0" xr:uid="{DAAD0B80-712C-C441-B2BC-853E4B577A79}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">rubric:
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> score: 1.5
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> type: formula
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B7" authorId="0" shapeId="0" xr:uid="{AAF9CEFF-2DF0-C340-9B67-76233EA5B21B}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">rubric:
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> score: 1
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> type: formula
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B8" authorId="0" shapeId="0" xr:uid="{3CCC1AE5-053B-C649-A73F-F4C7437CBDDA}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">rubric:
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> score: 1.5
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> type: formula
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B9" authorId="0" shapeId="0" xr:uid="{2DD28452-4D0F-454F-B08A-F896EE3CC1D5}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">rubric:
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> score: 1.5
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> type: formula
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">alt_cells:
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> - C10
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B11" authorId="0" shapeId="0" xr:uid="{B7712E80-D534-ED47-A1EA-2A5A08C12027}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">rubric:
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> score: 2
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> type: formula</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B12" authorId="0" shapeId="0" xr:uid="{A60AB632-FF04-DA42-9651-C4D1D0084018}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">rubric:
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> score: 2
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> type: formula</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments5.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Ricardo Pramana Suranta</author>
+  </authors>
+  <commentList>
     <comment ref="B5" authorId="0" shapeId="0" xr:uid="{2F37875C-F1FE-DB47-9444-CB9BC8E84C6F}">
       <text>
         <r>
@@ -1312,7 +1524,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="53">
   <si>
     <t>Number</t>
   </si>
@@ -1465,13 +1677,19 @@
   </si>
   <si>
     <t>// delta for being more tolerant</t>
+  </si>
+  <si>
+    <t>RelativeF Samples</t>
+  </si>
+  <si>
+    <t>// student is correct 3003 = 1001 + 2002 = 4004 - 1001</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1484,18 +1702,6 @@
       <color rgb="FF000000"/>
       <name val="Tahoma"/>
       <family val="2"/>
-    </font>
-    <font>
-      <sz val="18"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <sz val="18"/>
@@ -1545,10 +1751,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1848,10 +2050,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{713B2A36-CAF8-2349-917C-6D8074132DA3}">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:B5"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1899,6 +2101,178 @@
         <v>39</v>
       </c>
     </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>51</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{064C43C6-5CB5-C440-9F78-B7711421521C}">
+  <dimension ref="A1:E11"/>
+  <sheetViews>
+    <sheetView zoomScale="187" zoomScaleNormal="187" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="15.1640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2">
+        <v>2020</v>
+      </c>
+      <c r="E2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3">
+        <f>B2 / 10</f>
+        <v>202</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>31</v>
+      </c>
+      <c r="B4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5">
+        <f xml:space="preserve">  ROUNDUP(B2 / 100, B4)</f>
+        <v>21</v>
+      </c>
+      <c r="E5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8">
+        <f xml:space="preserve"> B7 / 1000</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9">
+        <f>B7 * 3.28084</f>
+        <v>3280.84</v>
+      </c>
+      <c r="E9" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10">
+        <f>B7 * 39.3701</f>
+        <v>39370.1</v>
+      </c>
+      <c r="E10" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C11">
+        <f>B7 * 39.37</f>
+        <v>39370</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8290A36-E311-014F-BFC1-47B09A169C19}">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>34</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1909,7 +2283,7 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection sqref="A1:B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1968,11 +2342,160 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B46F8006-805A-2247-9212-CACA8E8D41A6}">
+  <dimension ref="A1:B6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>46</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7CF2EB7E-182E-C148-9132-E2AAE2C42630}">
+  <dimension ref="A1:F10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I12" sqref="I12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <f>B2+C2</f>
+        <v>300</v>
+      </c>
+      <c r="B2">
+        <v>100</v>
+      </c>
+      <c r="C2">
+        <v>200</v>
+      </c>
+      <c r="D2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <f>B3+C3</f>
+        <v>300</v>
+      </c>
+      <c r="B3">
+        <v>100</v>
+      </c>
+      <c r="C3">
+        <v>200</v>
+      </c>
+      <c r="D3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <f>B4+C4</f>
+        <v>300</v>
+      </c>
+      <c r="B4">
+        <v>100</v>
+      </c>
+      <c r="C4">
+        <v>200</v>
+      </c>
+      <c r="D4" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <f>B5+C5</f>
+        <v>300</v>
+      </c>
+      <c r="B5">
+        <v>100</v>
+      </c>
+      <c r="C5">
+        <v>200</v>
+      </c>
+      <c r="D5" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F10">
+        <v>8888</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B5E91EC-3DFF-1543-8E9D-3526C440EDB3}">
   <dimension ref="A1:F10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2072,7 +2595,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A103586-2C0E-0748-80AF-98E299C769E5}">
   <dimension ref="A1:E10"/>
   <sheetViews>
@@ -2180,7 +2703,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71EABA77-C8A8-0247-A6AC-2452B8B329D1}">
   <dimension ref="A1:B8"/>
   <sheetViews>
@@ -2260,7 +2783,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EEB70C9E-5A32-AF4F-951C-2DFC686CB197}">
   <dimension ref="A1:E12"/>
   <sheetViews>
@@ -2383,7 +2906,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9AF83535-20BE-CA43-B82B-2F0E1F118D83}">
   <dimension ref="A1:C9"/>
   <sheetViews>
@@ -2472,168 +2995,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{064C43C6-5CB5-C440-9F78-B7711421521C}">
-  <dimension ref="A1:E11"/>
-  <sheetViews>
-    <sheetView zoomScale="187" zoomScaleNormal="187" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="15.1640625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2">
-        <v>2020</v>
-      </c>
-      <c r="E2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3">
-        <f>B2 / 10</f>
-        <v>202</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>31</v>
-      </c>
-      <c r="B4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5">
-        <f xml:space="preserve">  ROUNDUP(B2 / 100, B4)</f>
-        <v>21</v>
-      </c>
-      <c r="E5" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>11</v>
-      </c>
-      <c r="B7">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>12</v>
-      </c>
-      <c r="B8">
-        <f xml:space="preserve"> B7 / 1000</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>13</v>
-      </c>
-      <c r="B9">
-        <f>B7 * 3.28084</f>
-        <v>3280.84</v>
-      </c>
-      <c r="E9" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>14</v>
-      </c>
-      <c r="B10">
-        <f>B7 * 39.3701</f>
-        <v>39370.1</v>
-      </c>
-      <c r="E10" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="C11">
-        <f>B7 * 39.37</f>
-        <v>39370</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8290A36-E311-014F-BFC1-47B09A169C19}">
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>34</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>